<commit_message>
Aggiunto studio (da completare) sui nodi non-target
</commit_message>
<xml_diff>
--- a/analysis/test-dijkstra-dualascent.xlsx
+++ b/analysis/test-dijkstra-dualascent.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\anaws\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455852F9-AE64-46A0-87AC-E98CB00CA7BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC023198-B3DB-4610-8029-4626A5C78D47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{4FF27154-4CE8-4227-97A9-9900F5A89FA9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{4FF27154-4CE8-4227-97A9-9900F5A89FA9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Latenza" sheetId="1" r:id="rId1"/>
-    <sheet name="Banda EQ Dijkstra" sheetId="3" r:id="rId2"/>
-    <sheet name="Banda EQ Dual Ascent" sheetId="4" r:id="rId3"/>
-    <sheet name="Banda DIV Dijkstra" sheetId="5" r:id="rId4"/>
-    <sheet name="Banda DIV Dual Ascent" sheetId="6" r:id="rId5"/>
-    <sheet name="Target" sheetId="7" r:id="rId6"/>
+    <sheet name="Latenza all" sheetId="1" r:id="rId1"/>
+    <sheet name="Latenza Target" sheetId="7" r:id="rId2"/>
+    <sheet name="Banda EQ Dijkstra" sheetId="3" r:id="rId3"/>
+    <sheet name="Banda EQ Dual Ascent" sheetId="4" r:id="rId4"/>
+    <sheet name="Banda DIV Dijkstra" sheetId="5" r:id="rId5"/>
+    <sheet name="Banda DIV Dual Ascent" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="42">
   <si>
     <t>Mean</t>
   </si>
@@ -156,18 +156,6 @@
   </si>
   <si>
     <t>Nodes</t>
-  </si>
-  <si>
-    <t>h1-h14</t>
-  </si>
-  <si>
-    <t>h6-h14</t>
-  </si>
-  <si>
-    <t>h14-h1</t>
-  </si>
-  <si>
-    <t>h14-h6</t>
   </si>
   <si>
     <t>Average</t>
@@ -371,7 +359,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -489,9 +477,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -533,6 +518,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -570,6 +561,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -752,7 +747,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$B$5</c:f>
+              <c:f>'Latenza all'!$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -862,7 +857,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$E$5</c:f>
+              <c:f>'Latenza all'!$E$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -972,7 +967,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$C$5</c:f>
+              <c:f>'Latenza all'!$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1082,7 +1077,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$F$5</c:f>
+              <c:f>'Latenza all'!$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1192,7 +1187,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$D$5</c:f>
+              <c:f>'Latenza all'!$D$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1302,7 +1297,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$G$5</c:f>
+              <c:f>'Latenza all'!$G$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1593,7 +1588,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$B$7</c:f>
+              <c:f>'Latenza all'!$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1640,7 +1635,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$E$7</c:f>
+              <c:f>'Latenza all'!$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1687,7 +1682,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$C$7</c:f>
+              <c:f>'Latenza all'!$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1734,7 +1729,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$F$7</c:f>
+              <c:f>'Latenza all'!$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1781,7 +1776,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$D$7</c:f>
+              <c:f>'Latenza all'!$D$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1828,7 +1823,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Latenza!$G$7</c:f>
+              <c:f>'Latenza all'!$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -15704,7 +15699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF34C271-DF05-470A-888F-D3E261F22D54}">
   <dimension ref="A1:H407"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -15718,16 +15713,16 @@
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="60"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="59" t="s">
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="61"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="62"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
@@ -20268,6 +20263,1823 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F1448B-9046-4895-AF26-0705232310C8}">
+  <dimension ref="A1:P46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="72"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="71" t="s">
+        <v>37</v>
+      </c>
+      <c r="K1" s="71"/>
+      <c r="L1" s="71"/>
+      <c r="M1" s="71"/>
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="72"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="43"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="3"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="13"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="49"/>
+      <c r="B4" s="50">
+        <v>103</v>
+      </c>
+      <c r="C4" s="29">
+        <v>59</v>
+      </c>
+      <c r="D4" s="59">
+        <v>148</v>
+      </c>
+      <c r="E4" s="50">
+        <v>59</v>
+      </c>
+      <c r="F4" s="29">
+        <v>148</v>
+      </c>
+      <c r="G4" s="58">
+        <v>103</v>
+      </c>
+      <c r="I4" s="35"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="50">
+        <v>146</v>
+      </c>
+      <c r="L4" s="29">
+        <v>188</v>
+      </c>
+      <c r="M4" s="29">
+        <v>174</v>
+      </c>
+      <c r="N4" s="29">
+        <v>188</v>
+      </c>
+      <c r="O4" s="29">
+        <v>174</v>
+      </c>
+      <c r="P4" s="29">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="49"/>
+      <c r="B5" s="51">
+        <v>130</v>
+      </c>
+      <c r="C5" s="58">
+        <v>107</v>
+      </c>
+      <c r="D5" s="58">
+        <v>169</v>
+      </c>
+      <c r="E5" s="58">
+        <v>107</v>
+      </c>
+      <c r="F5" s="58">
+        <v>169</v>
+      </c>
+      <c r="G5" s="58">
+        <v>130</v>
+      </c>
+      <c r="I5" s="35"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="51">
+        <v>36</v>
+      </c>
+      <c r="L5" s="58">
+        <v>188</v>
+      </c>
+      <c r="M5" s="58">
+        <v>58</v>
+      </c>
+      <c r="N5" s="58">
+        <v>188</v>
+      </c>
+      <c r="O5" s="58">
+        <v>58</v>
+      </c>
+      <c r="P5" s="58">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="49"/>
+      <c r="B6" s="51">
+        <v>158</v>
+      </c>
+      <c r="C6" s="58">
+        <v>180</v>
+      </c>
+      <c r="D6" s="58">
+        <v>202</v>
+      </c>
+      <c r="E6" s="58">
+        <v>180</v>
+      </c>
+      <c r="F6" s="58">
+        <v>202</v>
+      </c>
+      <c r="G6" s="58">
+        <v>158</v>
+      </c>
+      <c r="I6" s="35"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="51">
+        <v>167</v>
+      </c>
+      <c r="L6" s="58">
+        <v>210</v>
+      </c>
+      <c r="M6" s="58">
+        <v>109</v>
+      </c>
+      <c r="N6" s="58">
+        <v>210</v>
+      </c>
+      <c r="O6" s="58">
+        <v>109</v>
+      </c>
+      <c r="P6" s="58">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="51">
+        <v>221</v>
+      </c>
+      <c r="C7" s="58">
+        <v>243</v>
+      </c>
+      <c r="D7" s="58">
+        <v>262</v>
+      </c>
+      <c r="E7" s="58">
+        <v>243</v>
+      </c>
+      <c r="F7" s="58">
+        <v>262</v>
+      </c>
+      <c r="G7" s="58">
+        <v>221</v>
+      </c>
+      <c r="I7" s="35"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="51">
+        <v>250</v>
+      </c>
+      <c r="L7" s="58">
+        <v>282</v>
+      </c>
+      <c r="M7" s="58">
+        <v>366</v>
+      </c>
+      <c r="N7" s="58">
+        <v>282</v>
+      </c>
+      <c r="O7" s="58">
+        <v>366</v>
+      </c>
+      <c r="P7" s="58">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="51">
+        <v>221</v>
+      </c>
+      <c r="C8" s="58">
+        <v>254</v>
+      </c>
+      <c r="D8" s="58">
+        <v>257</v>
+      </c>
+      <c r="E8" s="58">
+        <v>254</v>
+      </c>
+      <c r="F8" s="58">
+        <v>257</v>
+      </c>
+      <c r="G8" s="58">
+        <v>221</v>
+      </c>
+      <c r="I8" s="35"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="51">
+        <v>316</v>
+      </c>
+      <c r="L8" s="58">
+        <v>288</v>
+      </c>
+      <c r="M8" s="58">
+        <v>408</v>
+      </c>
+      <c r="N8" s="58">
+        <v>288</v>
+      </c>
+      <c r="O8" s="58">
+        <v>408</v>
+      </c>
+      <c r="P8" s="58">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="20"/>
+      <c r="B9" s="51">
+        <v>221</v>
+      </c>
+      <c r="C9" s="58">
+        <v>254</v>
+      </c>
+      <c r="D9" s="58">
+        <v>257</v>
+      </c>
+      <c r="E9" s="58">
+        <v>254</v>
+      </c>
+      <c r="F9" s="58">
+        <v>257</v>
+      </c>
+      <c r="G9" s="58">
+        <v>221</v>
+      </c>
+      <c r="I9" s="35"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="51">
+        <v>316</v>
+      </c>
+      <c r="L9" s="58">
+        <v>288</v>
+      </c>
+      <c r="M9" s="58">
+        <v>408</v>
+      </c>
+      <c r="N9" s="58">
+        <v>288</v>
+      </c>
+      <c r="O9" s="58">
+        <v>408</v>
+      </c>
+      <c r="P9" s="58">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A10" s="20"/>
+      <c r="B10" s="51">
+        <v>221</v>
+      </c>
+      <c r="C10" s="58">
+        <v>254</v>
+      </c>
+      <c r="D10" s="58">
+        <v>257</v>
+      </c>
+      <c r="E10" s="58">
+        <v>254</v>
+      </c>
+      <c r="F10" s="58">
+        <v>257</v>
+      </c>
+      <c r="G10" s="58">
+        <v>221</v>
+      </c>
+      <c r="I10" s="35"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="51">
+        <v>316</v>
+      </c>
+      <c r="L10" s="58">
+        <v>270</v>
+      </c>
+      <c r="M10" s="58">
+        <v>410</v>
+      </c>
+      <c r="N10" s="58">
+        <v>270</v>
+      </c>
+      <c r="O10" s="58">
+        <v>410</v>
+      </c>
+      <c r="P10" s="58">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A11" s="20"/>
+      <c r="B11" s="51">
+        <v>221</v>
+      </c>
+      <c r="C11" s="58">
+        <v>254</v>
+      </c>
+      <c r="D11" s="58">
+        <v>257</v>
+      </c>
+      <c r="E11" s="58">
+        <v>254</v>
+      </c>
+      <c r="F11" s="58">
+        <v>257</v>
+      </c>
+      <c r="G11" s="58">
+        <v>221</v>
+      </c>
+      <c r="I11" s="35"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="51">
+        <v>369</v>
+      </c>
+      <c r="L11" s="58">
+        <v>270</v>
+      </c>
+      <c r="M11" s="58">
+        <v>320</v>
+      </c>
+      <c r="N11" s="58">
+        <v>270</v>
+      </c>
+      <c r="O11" s="58">
+        <v>320</v>
+      </c>
+      <c r="P11" s="58">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A12" s="20"/>
+      <c r="B12" s="51">
+        <v>221</v>
+      </c>
+      <c r="C12" s="58">
+        <v>254</v>
+      </c>
+      <c r="D12" s="58">
+        <v>257</v>
+      </c>
+      <c r="E12" s="58">
+        <v>254</v>
+      </c>
+      <c r="F12" s="58">
+        <v>257</v>
+      </c>
+      <c r="G12" s="58">
+        <v>221</v>
+      </c>
+      <c r="I12" s="35"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="51">
+        <v>349</v>
+      </c>
+      <c r="L12" s="58">
+        <v>285</v>
+      </c>
+      <c r="M12" s="58">
+        <v>185</v>
+      </c>
+      <c r="N12" s="58">
+        <v>285</v>
+      </c>
+      <c r="O12" s="58">
+        <v>185</v>
+      </c>
+      <c r="P12" s="58">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="20"/>
+      <c r="B13" s="51">
+        <v>207</v>
+      </c>
+      <c r="C13" s="58">
+        <v>240</v>
+      </c>
+      <c r="D13" s="58">
+        <v>257</v>
+      </c>
+      <c r="E13" s="58">
+        <v>240</v>
+      </c>
+      <c r="F13" s="58">
+        <v>257</v>
+      </c>
+      <c r="G13" s="58">
+        <v>207</v>
+      </c>
+      <c r="I13" s="35"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="51">
+        <v>335</v>
+      </c>
+      <c r="L13" s="58">
+        <v>285</v>
+      </c>
+      <c r="M13" s="58">
+        <v>171</v>
+      </c>
+      <c r="N13" s="58">
+        <v>285</v>
+      </c>
+      <c r="O13" s="58">
+        <v>171</v>
+      </c>
+      <c r="P13" s="58">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A14" s="20"/>
+      <c r="B14" s="51">
+        <v>207</v>
+      </c>
+      <c r="C14" s="58">
+        <v>240</v>
+      </c>
+      <c r="D14" s="58">
+        <v>257</v>
+      </c>
+      <c r="E14" s="58">
+        <v>240</v>
+      </c>
+      <c r="F14" s="58">
+        <v>257</v>
+      </c>
+      <c r="G14" s="58">
+        <v>207</v>
+      </c>
+      <c r="I14" s="35"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="51">
+        <v>431</v>
+      </c>
+      <c r="L14" s="58">
+        <v>308</v>
+      </c>
+      <c r="M14" s="58">
+        <v>281</v>
+      </c>
+      <c r="N14" s="58">
+        <v>308</v>
+      </c>
+      <c r="O14" s="58">
+        <v>281</v>
+      </c>
+      <c r="P14" s="58">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="51">
+        <v>207</v>
+      </c>
+      <c r="C15" s="58">
+        <v>240</v>
+      </c>
+      <c r="D15" s="58">
+        <v>257</v>
+      </c>
+      <c r="E15" s="58">
+        <v>240</v>
+      </c>
+      <c r="F15" s="58">
+        <v>257</v>
+      </c>
+      <c r="G15" s="58">
+        <v>207</v>
+      </c>
+      <c r="I15" s="35"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="51">
+        <v>380</v>
+      </c>
+      <c r="L15" s="58">
+        <v>279</v>
+      </c>
+      <c r="M15" s="58">
+        <v>252</v>
+      </c>
+      <c r="N15" s="58">
+        <v>279</v>
+      </c>
+      <c r="O15" s="58">
+        <v>252</v>
+      </c>
+      <c r="P15" s="58">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A16" s="20"/>
+      <c r="B16" s="51">
+        <v>176</v>
+      </c>
+      <c r="C16" s="58">
+        <v>187</v>
+      </c>
+      <c r="D16" s="58">
+        <v>243</v>
+      </c>
+      <c r="E16" s="58">
+        <v>187</v>
+      </c>
+      <c r="F16" s="58">
+        <v>243</v>
+      </c>
+      <c r="G16" s="58">
+        <v>176</v>
+      </c>
+      <c r="I16" s="35"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="51">
+        <v>304</v>
+      </c>
+      <c r="L16" s="58">
+        <v>299</v>
+      </c>
+      <c r="M16" s="58">
+        <v>392</v>
+      </c>
+      <c r="N16" s="58">
+        <v>299</v>
+      </c>
+      <c r="O16" s="58">
+        <v>392</v>
+      </c>
+      <c r="P16" s="58">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A17" s="20"/>
+      <c r="B17" s="51">
+        <v>176</v>
+      </c>
+      <c r="C17" s="58">
+        <v>187</v>
+      </c>
+      <c r="D17" s="58">
+        <v>243</v>
+      </c>
+      <c r="E17" s="58">
+        <v>187</v>
+      </c>
+      <c r="F17" s="58">
+        <v>243</v>
+      </c>
+      <c r="G17" s="58">
+        <v>176</v>
+      </c>
+      <c r="I17" s="35"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="51">
+        <v>304</v>
+      </c>
+      <c r="L17" s="58">
+        <v>299</v>
+      </c>
+      <c r="M17" s="58">
+        <v>392</v>
+      </c>
+      <c r="N17" s="58">
+        <v>299</v>
+      </c>
+      <c r="O17" s="58">
+        <v>392</v>
+      </c>
+      <c r="P17" s="58">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="20"/>
+      <c r="B18" s="51">
+        <v>220</v>
+      </c>
+      <c r="C18" s="58">
+        <v>231</v>
+      </c>
+      <c r="D18" s="58">
+        <v>243</v>
+      </c>
+      <c r="E18" s="58">
+        <v>231</v>
+      </c>
+      <c r="F18" s="58">
+        <v>243</v>
+      </c>
+      <c r="G18" s="58">
+        <v>220</v>
+      </c>
+      <c r="I18" s="35"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="51">
+        <v>403</v>
+      </c>
+      <c r="L18" s="58">
+        <v>229</v>
+      </c>
+      <c r="M18" s="58">
+        <v>234</v>
+      </c>
+      <c r="N18" s="58">
+        <v>229</v>
+      </c>
+      <c r="O18" s="58">
+        <v>234</v>
+      </c>
+      <c r="P18" s="58">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
+      <c r="B19" s="51">
+        <v>234</v>
+      </c>
+      <c r="C19" s="58">
+        <v>231</v>
+      </c>
+      <c r="D19" s="58">
+        <v>243</v>
+      </c>
+      <c r="E19" s="58">
+        <v>231</v>
+      </c>
+      <c r="F19" s="58">
+        <v>243</v>
+      </c>
+      <c r="G19" s="58">
+        <v>234</v>
+      </c>
+      <c r="I19" s="35"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="51">
+        <v>163</v>
+      </c>
+      <c r="L19" s="58">
+        <v>229</v>
+      </c>
+      <c r="M19" s="58">
+        <v>218</v>
+      </c>
+      <c r="N19" s="58">
+        <v>229</v>
+      </c>
+      <c r="O19" s="58">
+        <v>218</v>
+      </c>
+      <c r="P19" s="58">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
+      <c r="B20" s="51">
+        <v>246</v>
+      </c>
+      <c r="C20" s="58">
+        <v>243</v>
+      </c>
+      <c r="D20" s="58">
+        <v>257</v>
+      </c>
+      <c r="E20" s="58">
+        <v>243</v>
+      </c>
+      <c r="F20" s="58">
+        <v>257</v>
+      </c>
+      <c r="G20" s="58">
+        <v>246</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="51">
+        <v>163</v>
+      </c>
+      <c r="L20" s="58">
+        <v>229</v>
+      </c>
+      <c r="M20" s="58">
+        <v>218</v>
+      </c>
+      <c r="N20" s="58">
+        <v>229</v>
+      </c>
+      <c r="O20" s="58">
+        <v>218</v>
+      </c>
+      <c r="P20" s="58">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="20"/>
+      <c r="B21" s="51">
+        <v>246</v>
+      </c>
+      <c r="C21" s="58">
+        <v>253</v>
+      </c>
+      <c r="D21" s="58">
+        <v>267</v>
+      </c>
+      <c r="E21" s="58">
+        <v>253</v>
+      </c>
+      <c r="F21" s="58">
+        <v>267</v>
+      </c>
+      <c r="G21" s="58">
+        <v>246</v>
+      </c>
+      <c r="I21" s="35"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="51">
+        <v>292</v>
+      </c>
+      <c r="L21" s="58">
+        <v>209</v>
+      </c>
+      <c r="M21" s="58">
+        <v>218</v>
+      </c>
+      <c r="N21" s="58">
+        <v>209</v>
+      </c>
+      <c r="O21" s="58">
+        <v>218</v>
+      </c>
+      <c r="P21" s="58">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="20"/>
+      <c r="B22" s="51">
+        <v>246</v>
+      </c>
+      <c r="C22" s="58">
+        <v>253</v>
+      </c>
+      <c r="D22" s="58">
+        <v>267</v>
+      </c>
+      <c r="E22" s="58">
+        <v>253</v>
+      </c>
+      <c r="F22" s="58">
+        <v>267</v>
+      </c>
+      <c r="G22" s="58">
+        <v>246</v>
+      </c>
+      <c r="I22" s="35"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="51">
+        <v>285</v>
+      </c>
+      <c r="L22" s="58">
+        <v>209</v>
+      </c>
+      <c r="M22" s="58">
+        <v>218</v>
+      </c>
+      <c r="N22" s="58">
+        <v>209</v>
+      </c>
+      <c r="O22" s="58">
+        <v>218</v>
+      </c>
+      <c r="P22" s="58">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="20"/>
+      <c r="B23" s="51">
+        <v>246</v>
+      </c>
+      <c r="C23" s="58">
+        <v>253</v>
+      </c>
+      <c r="D23" s="58">
+        <v>267</v>
+      </c>
+      <c r="E23" s="58">
+        <v>253</v>
+      </c>
+      <c r="F23" s="58">
+        <v>267</v>
+      </c>
+      <c r="G23" s="58">
+        <v>246</v>
+      </c>
+      <c r="I23" s="35"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="51">
+        <v>285</v>
+      </c>
+      <c r="L23" s="58">
+        <v>209</v>
+      </c>
+      <c r="M23" s="58">
+        <v>218</v>
+      </c>
+      <c r="N23" s="58">
+        <v>209</v>
+      </c>
+      <c r="O23" s="58">
+        <v>218</v>
+      </c>
+      <c r="P23" s="58">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="20"/>
+      <c r="B24" s="51">
+        <v>246</v>
+      </c>
+      <c r="C24" s="58">
+        <v>253</v>
+      </c>
+      <c r="D24" s="58">
+        <v>267</v>
+      </c>
+      <c r="E24" s="58">
+        <v>253</v>
+      </c>
+      <c r="F24" s="58">
+        <v>267</v>
+      </c>
+      <c r="G24" s="58">
+        <v>246</v>
+      </c>
+      <c r="I24" s="35"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="51">
+        <v>285</v>
+      </c>
+      <c r="L24" s="58">
+        <v>209</v>
+      </c>
+      <c r="M24" s="58">
+        <v>220</v>
+      </c>
+      <c r="N24" s="58">
+        <v>209</v>
+      </c>
+      <c r="O24" s="58">
+        <v>220</v>
+      </c>
+      <c r="P24" s="58">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="20"/>
+      <c r="B25" s="51">
+        <v>246</v>
+      </c>
+      <c r="C25" s="58">
+        <v>253</v>
+      </c>
+      <c r="D25" s="58">
+        <v>267</v>
+      </c>
+      <c r="E25" s="58">
+        <v>253</v>
+      </c>
+      <c r="F25" s="58">
+        <v>267</v>
+      </c>
+      <c r="G25" s="58">
+        <v>246</v>
+      </c>
+      <c r="I25" s="35"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="51">
+        <v>285</v>
+      </c>
+      <c r="L25" s="58">
+        <v>209</v>
+      </c>
+      <c r="M25" s="58">
+        <v>220</v>
+      </c>
+      <c r="N25" s="58">
+        <v>209</v>
+      </c>
+      <c r="O25" s="58">
+        <v>220</v>
+      </c>
+      <c r="P25" s="58">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="20"/>
+      <c r="B26" s="51">
+        <v>232</v>
+      </c>
+      <c r="C26" s="58">
+        <v>239</v>
+      </c>
+      <c r="D26" s="58">
+        <v>267</v>
+      </c>
+      <c r="E26" s="58">
+        <v>239</v>
+      </c>
+      <c r="F26" s="58">
+        <v>267</v>
+      </c>
+      <c r="G26" s="58">
+        <v>232</v>
+      </c>
+      <c r="I26" s="35"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="51">
+        <v>333</v>
+      </c>
+      <c r="L26" s="58">
+        <v>242</v>
+      </c>
+      <c r="M26" s="58">
+        <v>220</v>
+      </c>
+      <c r="N26" s="58">
+        <v>242</v>
+      </c>
+      <c r="O26" s="58">
+        <v>220</v>
+      </c>
+      <c r="P26" s="58">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="20"/>
+      <c r="B27" s="51">
+        <v>232</v>
+      </c>
+      <c r="C27" s="58">
+        <v>239</v>
+      </c>
+      <c r="D27" s="58">
+        <v>267</v>
+      </c>
+      <c r="E27" s="58">
+        <v>239</v>
+      </c>
+      <c r="F27" s="58">
+        <v>267</v>
+      </c>
+      <c r="G27" s="58">
+        <v>232</v>
+      </c>
+      <c r="I27" s="35"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="51">
+        <v>340</v>
+      </c>
+      <c r="L27" s="58">
+        <v>242</v>
+      </c>
+      <c r="M27" s="58">
+        <v>218</v>
+      </c>
+      <c r="N27" s="58">
+        <v>242</v>
+      </c>
+      <c r="O27" s="58">
+        <v>218</v>
+      </c>
+      <c r="P27" s="58">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="20"/>
+      <c r="B28" s="51">
+        <v>243</v>
+      </c>
+      <c r="C28" s="58">
+        <v>264</v>
+      </c>
+      <c r="D28" s="58">
+        <v>294</v>
+      </c>
+      <c r="E28" s="58">
+        <v>264</v>
+      </c>
+      <c r="F28" s="58">
+        <v>294</v>
+      </c>
+      <c r="G28" s="58">
+        <v>243</v>
+      </c>
+      <c r="I28" s="35"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="51">
+        <v>340</v>
+      </c>
+      <c r="L28" s="58">
+        <v>242</v>
+      </c>
+      <c r="M28" s="58">
+        <v>431</v>
+      </c>
+      <c r="N28" s="58">
+        <v>242</v>
+      </c>
+      <c r="O28" s="58">
+        <v>431</v>
+      </c>
+      <c r="P28" s="58">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="20"/>
+      <c r="B29" s="51">
+        <v>243</v>
+      </c>
+      <c r="C29" s="58">
+        <v>264</v>
+      </c>
+      <c r="D29" s="58">
+        <v>294</v>
+      </c>
+      <c r="E29" s="58">
+        <v>264</v>
+      </c>
+      <c r="F29" s="58">
+        <v>294</v>
+      </c>
+      <c r="G29" s="58">
+        <v>243</v>
+      </c>
+      <c r="I29" s="35"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="51">
+        <v>166</v>
+      </c>
+      <c r="L29" s="58">
+        <v>223</v>
+      </c>
+      <c r="M29" s="58">
+        <v>341</v>
+      </c>
+      <c r="N29" s="58">
+        <v>223</v>
+      </c>
+      <c r="O29" s="58">
+        <v>341</v>
+      </c>
+      <c r="P29" s="58">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="20"/>
+      <c r="B30" s="51">
+        <v>255</v>
+      </c>
+      <c r="C30" s="58">
+        <v>276</v>
+      </c>
+      <c r="D30" s="58">
+        <v>294</v>
+      </c>
+      <c r="E30" s="58">
+        <v>276</v>
+      </c>
+      <c r="F30" s="58">
+        <v>294</v>
+      </c>
+      <c r="G30" s="58">
+        <v>255</v>
+      </c>
+      <c r="I30" s="35"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="51">
+        <v>182</v>
+      </c>
+      <c r="L30" s="58">
+        <v>190</v>
+      </c>
+      <c r="M30" s="58">
+        <v>210</v>
+      </c>
+      <c r="N30" s="58">
+        <v>190</v>
+      </c>
+      <c r="O30" s="58">
+        <v>210</v>
+      </c>
+      <c r="P30" s="58">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="20"/>
+      <c r="B31" s="51">
+        <v>255</v>
+      </c>
+      <c r="C31" s="58">
+        <v>276</v>
+      </c>
+      <c r="D31" s="58">
+        <v>304</v>
+      </c>
+      <c r="E31" s="58">
+        <v>276</v>
+      </c>
+      <c r="F31" s="58">
+        <v>304</v>
+      </c>
+      <c r="G31" s="58">
+        <v>255</v>
+      </c>
+      <c r="I31" s="35"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="51">
+        <v>182</v>
+      </c>
+      <c r="L31" s="58">
+        <v>190</v>
+      </c>
+      <c r="M31" s="58">
+        <v>176</v>
+      </c>
+      <c r="N31" s="58">
+        <v>190</v>
+      </c>
+      <c r="O31" s="58">
+        <v>176</v>
+      </c>
+      <c r="P31" s="58">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="20"/>
+      <c r="B32" s="51">
+        <v>255</v>
+      </c>
+      <c r="C32" s="58">
+        <v>276</v>
+      </c>
+      <c r="D32" s="58">
+        <v>304</v>
+      </c>
+      <c r="E32" s="58">
+        <v>276</v>
+      </c>
+      <c r="F32" s="58">
+        <v>304</v>
+      </c>
+      <c r="G32" s="58">
+        <v>255</v>
+      </c>
+      <c r="I32" s="35"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="51">
+        <v>182</v>
+      </c>
+      <c r="L32" s="58">
+        <v>218</v>
+      </c>
+      <c r="M32" s="58">
+        <v>148</v>
+      </c>
+      <c r="N32" s="58">
+        <v>218</v>
+      </c>
+      <c r="O32" s="58">
+        <v>148</v>
+      </c>
+      <c r="P32" s="58">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+      <c r="B33" s="51">
+        <v>255</v>
+      </c>
+      <c r="C33" s="58">
+        <v>276</v>
+      </c>
+      <c r="D33" s="58">
+        <v>304</v>
+      </c>
+      <c r="E33" s="58">
+        <v>276</v>
+      </c>
+      <c r="F33" s="58">
+        <v>304</v>
+      </c>
+      <c r="G33" s="58">
+        <v>255</v>
+      </c>
+      <c r="I33" s="35"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="51">
+        <v>157</v>
+      </c>
+      <c r="L33" s="58">
+        <v>162</v>
+      </c>
+      <c r="M33" s="58">
+        <v>148</v>
+      </c>
+      <c r="N33" s="58">
+        <v>162</v>
+      </c>
+      <c r="O33" s="58">
+        <v>148</v>
+      </c>
+      <c r="P33" s="58">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="20"/>
+      <c r="B34" s="51">
+        <v>255</v>
+      </c>
+      <c r="C34" s="58">
+        <v>276</v>
+      </c>
+      <c r="D34" s="58">
+        <v>304</v>
+      </c>
+      <c r="E34" s="58">
+        <v>276</v>
+      </c>
+      <c r="F34" s="58">
+        <v>304</v>
+      </c>
+      <c r="G34" s="58">
+        <v>255</v>
+      </c>
+      <c r="I34" s="35"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="51">
+        <v>167</v>
+      </c>
+      <c r="L34" s="58">
+        <v>203</v>
+      </c>
+      <c r="M34" s="58">
+        <v>148</v>
+      </c>
+      <c r="N34" s="58">
+        <v>203</v>
+      </c>
+      <c r="O34" s="58">
+        <v>148</v>
+      </c>
+      <c r="P34" s="58">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="20"/>
+      <c r="B35" s="51">
+        <v>239</v>
+      </c>
+      <c r="C35" s="58">
+        <v>260</v>
+      </c>
+      <c r="D35" s="58">
+        <v>304</v>
+      </c>
+      <c r="E35" s="58">
+        <v>260</v>
+      </c>
+      <c r="F35" s="58">
+        <v>304</v>
+      </c>
+      <c r="G35" s="58">
+        <v>239</v>
+      </c>
+      <c r="I35" s="35"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="51">
+        <v>143</v>
+      </c>
+      <c r="L35" s="58">
+        <v>179</v>
+      </c>
+      <c r="M35" s="58">
+        <v>148</v>
+      </c>
+      <c r="N35" s="58">
+        <v>179</v>
+      </c>
+      <c r="O35" s="58">
+        <v>148</v>
+      </c>
+      <c r="P35" s="58">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A36" s="20"/>
+      <c r="B36" s="51">
+        <v>239</v>
+      </c>
+      <c r="C36" s="58">
+        <v>260</v>
+      </c>
+      <c r="D36" s="58">
+        <v>304</v>
+      </c>
+      <c r="E36" s="58">
+        <v>260</v>
+      </c>
+      <c r="F36" s="58">
+        <v>304</v>
+      </c>
+      <c r="G36" s="58">
+        <v>239</v>
+      </c>
+      <c r="I36" s="35"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="51">
+        <v>143</v>
+      </c>
+      <c r="L36" s="58">
+        <v>205</v>
+      </c>
+      <c r="M36" s="58">
+        <v>148</v>
+      </c>
+      <c r="N36" s="58">
+        <v>205</v>
+      </c>
+      <c r="O36" s="58">
+        <v>148</v>
+      </c>
+      <c r="P36" s="58">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A37" s="20"/>
+      <c r="B37" s="51">
+        <v>262</v>
+      </c>
+      <c r="C37" s="58">
+        <v>272</v>
+      </c>
+      <c r="D37" s="58">
+        <v>304</v>
+      </c>
+      <c r="E37" s="58">
+        <v>272</v>
+      </c>
+      <c r="F37" s="58">
+        <v>304</v>
+      </c>
+      <c r="G37" s="58">
+        <v>262</v>
+      </c>
+      <c r="I37" s="35"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="51">
+        <v>346</v>
+      </c>
+      <c r="L37" s="58">
+        <v>293</v>
+      </c>
+      <c r="M37" s="58">
+        <v>417</v>
+      </c>
+      <c r="N37" s="58">
+        <v>293</v>
+      </c>
+      <c r="O37" s="58">
+        <v>417</v>
+      </c>
+      <c r="P37" s="58">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="22"/>
+      <c r="B38" s="52">
+        <v>262</v>
+      </c>
+      <c r="C38" s="3">
+        <v>272</v>
+      </c>
+      <c r="D38" s="3">
+        <v>304</v>
+      </c>
+      <c r="E38" s="3">
+        <v>272</v>
+      </c>
+      <c r="F38" s="3">
+        <v>304</v>
+      </c>
+      <c r="G38" s="3">
+        <v>262</v>
+      </c>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="52">
+        <v>346</v>
+      </c>
+      <c r="L38" s="3">
+        <v>319</v>
+      </c>
+      <c r="M38" s="3">
+        <v>417</v>
+      </c>
+      <c r="N38" s="3">
+        <v>319</v>
+      </c>
+      <c r="O38" s="3">
+        <v>417</v>
+      </c>
+      <c r="P38" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A39" s="20"/>
+      <c r="B39" s="51"/>
+      <c r="C39" s="51"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="58"/>
+      <c r="G39" s="42"/>
+      <c r="I39" s="35"/>
+      <c r="J39" s="20"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="58"/>
+      <c r="P39" s="42"/>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A40" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40" s="53">
+        <f>AVERAGE(B4:B38)</f>
+        <v>224.2</v>
+      </c>
+      <c r="C40" s="53">
+        <f>AVERAGE(C4:C38)</f>
+        <v>239.22857142857143</v>
+      </c>
+      <c r="D40" s="53">
+        <f>AVERAGE(D4:D38)</f>
+        <v>264.25714285714287</v>
+      </c>
+      <c r="E40" s="53">
+        <f>AVERAGE(E4:E38)</f>
+        <v>239.22857142857143</v>
+      </c>
+      <c r="F40" s="6">
+        <f>AVERAGE(F4:F38)</f>
+        <v>264.25714285714287</v>
+      </c>
+      <c r="G40" s="6">
+        <f>AVERAGE(G4:G38)</f>
+        <v>224.2</v>
+      </c>
+      <c r="H40" s="26"/>
+      <c r="I40" s="56"/>
+      <c r="J40" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K40" s="53">
+        <f>AVERAGE(K4:K38)</f>
+        <v>263.05714285714288</v>
+      </c>
+      <c r="L40" s="53">
+        <f>AVERAGE(L4:L38)</f>
+        <v>239.4</v>
+      </c>
+      <c r="M40" s="53">
+        <f>AVERAGE(M4:M38)</f>
+        <v>253.14285714285714</v>
+      </c>
+      <c r="N40" s="53">
+        <f>AVERAGE(N4:N38)</f>
+        <v>239.4</v>
+      </c>
+      <c r="O40" s="6">
+        <f>AVERAGE(O4:O38)</f>
+        <v>253.14285714285714</v>
+      </c>
+      <c r="P40" s="6">
+        <f>AVERAGE(P4:P38)</f>
+        <v>263.05714285714288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A41" s="23"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="53"/>
+      <c r="D41" s="53"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="56"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="53"/>
+      <c r="L41" s="53"/>
+      <c r="M41" s="53"/>
+      <c r="N41" s="53"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A42" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="53">
+        <f>_xlfn.STDEV.S(B4:B38)</f>
+        <v>36.531050451072801</v>
+      </c>
+      <c r="C42" s="53">
+        <f>_xlfn.STDEV.S(C4:C38)</f>
+        <v>46.060756369288221</v>
+      </c>
+      <c r="D42" s="53">
+        <f>_xlfn.STDEV.S(D4:D38)</f>
+        <v>36.012532832451626</v>
+      </c>
+      <c r="E42" s="53">
+        <f>_xlfn.STDEV.S(E4:E38)</f>
+        <v>46.060756369288221</v>
+      </c>
+      <c r="F42" s="6">
+        <f>_xlfn.STDEV.S(F4:F38)</f>
+        <v>36.012532832451626</v>
+      </c>
+      <c r="G42" s="6">
+        <f>_xlfn.STDEV.S(G4:G38)</f>
+        <v>36.531050451072801</v>
+      </c>
+      <c r="H42" s="26"/>
+      <c r="I42" s="56"/>
+      <c r="J42" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="K42" s="53">
+        <f>_xlfn.STDEV.S(K4:K38)</f>
+        <v>94.460991904577384</v>
+      </c>
+      <c r="L42" s="53">
+        <f>_xlfn.STDEV.S(L4:L38)</f>
+        <v>43.395039022504669</v>
+      </c>
+      <c r="M42" s="53">
+        <f>_xlfn.STDEV.S(M4:M38)</f>
+        <v>104.71730652434817</v>
+      </c>
+      <c r="N42" s="53">
+        <f>_xlfn.STDEV.S(N4:N38)</f>
+        <v>43.395039022504669</v>
+      </c>
+      <c r="O42" s="6">
+        <f>_xlfn.STDEV.S(O4:O38)</f>
+        <v>104.71730652434817</v>
+      </c>
+      <c r="P42" s="6">
+        <f>_xlfn.STDEV.S(P4:P38)</f>
+        <v>94.460991904577384</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A43" s="23"/>
+      <c r="B43" s="53"/>
+      <c r="C43" s="53"/>
+      <c r="D43" s="53"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="56"/>
+      <c r="J43" s="23"/>
+      <c r="K43" s="53"/>
+      <c r="L43" s="53"/>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="6"/>
+    </row>
+    <row r="44" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="54">
+        <f>_xlfn.CONFIDENCE.NORM(0.05,B42,35)</f>
+        <v>12.102531714676296</v>
+      </c>
+      <c r="C44" s="54">
+        <f t="shared" ref="C44:G44" si="0">_xlfn.CONFIDENCE.NORM(0.05,C42,35)</f>
+        <v>15.259669729670156</v>
+      </c>
+      <c r="D44" s="54">
+        <f t="shared" si="0"/>
+        <v>11.930749741628848</v>
+      </c>
+      <c r="E44" s="54">
+        <f t="shared" si="0"/>
+        <v>15.259669729670156</v>
+      </c>
+      <c r="F44" s="54">
+        <f t="shared" si="0"/>
+        <v>11.930749741628848</v>
+      </c>
+      <c r="G44" s="8">
+        <f t="shared" si="0"/>
+        <v>12.102531714676296</v>
+      </c>
+      <c r="H44" s="26"/>
+      <c r="I44" s="56"/>
+      <c r="J44" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="K44" s="54">
+        <f>_xlfn.CONFIDENCE.NORM(0.05,K42,40)</f>
+        <v>29.273226764509225</v>
+      </c>
+      <c r="L44" s="54">
+        <f t="shared" ref="L44:P44" si="1">_xlfn.CONFIDENCE.NORM(0.05,L42,40)</f>
+        <v>13.448014806405492</v>
+      </c>
+      <c r="M44" s="54">
+        <f t="shared" si="1"/>
+        <v>32.451633190052519</v>
+      </c>
+      <c r="N44" s="54">
+        <f t="shared" si="1"/>
+        <v>13.448014806405492</v>
+      </c>
+      <c r="O44" s="8">
+        <f t="shared" si="1"/>
+        <v>32.451633190052519</v>
+      </c>
+      <c r="P44" s="8">
+        <f t="shared" si="1"/>
+        <v>29.273226764509225</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" s="23"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+    </row>
+    <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="8">
+        <f>AVERAGE(B40:G40)</f>
+        <v>242.56190476190477</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="K46" s="8">
+        <f>AVERAGE(K40:P40)</f>
+        <v>251.86666666666667</v>
+      </c>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="J1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E741BD8E-F329-4A9D-BAC2-C03CF5D0EF3C}">
   <dimension ref="A1:CS46"/>
   <sheetViews>
@@ -20296,114 +22108,114 @@
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="68" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="63" t="s">
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="64"/>
-      <c r="AJ1" s="64"/>
-      <c r="AK1" s="64"/>
-      <c r="AL1" s="64"/>
-      <c r="AM1" s="64"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
-      <c r="AP1" s="64"/>
-      <c r="AQ1" s="64"/>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="65"/>
-      <c r="AX1" s="66" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="66"/>
+      <c r="AX1" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="AY1" s="66"/>
-      <c r="AZ1" s="66"/>
-      <c r="BA1" s="66"/>
-      <c r="BB1" s="66"/>
-      <c r="BC1" s="66"/>
-      <c r="BD1" s="66"/>
-      <c r="BE1" s="66"/>
-      <c r="BF1" s="66"/>
-      <c r="BG1" s="66"/>
-      <c r="BH1" s="66"/>
-      <c r="BI1" s="66"/>
-      <c r="BJ1" s="66"/>
-      <c r="BK1" s="66"/>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="66" t="s">
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="67"/>
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="BO1" s="66"/>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="66"/>
-      <c r="BR1" s="66"/>
-      <c r="BS1" s="66"/>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="66"/>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="66"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="67"/>
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="67"/>
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="66"/>
-      <c r="CH1" s="66"/>
-      <c r="CI1" s="66"/>
-      <c r="CJ1" s="66"/>
-      <c r="CK1" s="66"/>
-      <c r="CL1" s="66"/>
-      <c r="CM1" s="66"/>
-      <c r="CN1" s="66"/>
-      <c r="CO1" s="66"/>
-      <c r="CP1" s="66"/>
-      <c r="CQ1" s="66"/>
-      <c r="CR1" s="66"/>
-      <c r="CS1" s="67"/>
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="67"/>
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="67"/>
+      <c r="CS1" s="68"/>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" s="12"/>
@@ -31125,7 +32937,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5F24C38-3DA2-4AE0-B9BB-0958C9CC608A}">
   <dimension ref="A1:CS46"/>
   <sheetViews>
@@ -31154,114 +32966,114 @@
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="68" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="63" t="s">
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="64"/>
-      <c r="AJ1" s="64"/>
-      <c r="AK1" s="64"/>
-      <c r="AL1" s="64"/>
-      <c r="AM1" s="64"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
-      <c r="AP1" s="64"/>
-      <c r="AQ1" s="64"/>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="65"/>
-      <c r="AX1" s="66" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="66"/>
+      <c r="AX1" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="AY1" s="66"/>
-      <c r="AZ1" s="66"/>
-      <c r="BA1" s="66"/>
-      <c r="BB1" s="66"/>
-      <c r="BC1" s="66"/>
-      <c r="BD1" s="66"/>
-      <c r="BE1" s="66"/>
-      <c r="BF1" s="66"/>
-      <c r="BG1" s="66"/>
-      <c r="BH1" s="66"/>
-      <c r="BI1" s="66"/>
-      <c r="BJ1" s="66"/>
-      <c r="BK1" s="66"/>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="66" t="s">
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="67"/>
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="BO1" s="66"/>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="66"/>
-      <c r="BR1" s="66"/>
-      <c r="BS1" s="66"/>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="66"/>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="66"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="67"/>
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="67"/>
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="66"/>
-      <c r="CH1" s="66"/>
-      <c r="CI1" s="66"/>
-      <c r="CJ1" s="66"/>
-      <c r="CK1" s="66"/>
-      <c r="CL1" s="66"/>
-      <c r="CM1" s="66"/>
-      <c r="CN1" s="66"/>
-      <c r="CO1" s="66"/>
-      <c r="CP1" s="66"/>
-      <c r="CQ1" s="66"/>
-      <c r="CR1" s="66"/>
-      <c r="CS1" s="67"/>
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="67"/>
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="67"/>
+      <c r="CS1" s="68"/>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" s="16"/>
@@ -42156,7 +43968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BD29032-954F-457A-A856-7615B2A12CA7}">
   <dimension ref="A1:CS43"/>
   <sheetViews>
@@ -42185,114 +43997,114 @@
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="68" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="63" t="s">
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="64"/>
-      <c r="AJ1" s="64"/>
-      <c r="AK1" s="64"/>
-      <c r="AL1" s="64"/>
-      <c r="AM1" s="64"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
-      <c r="AP1" s="64"/>
-      <c r="AQ1" s="64"/>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="65"/>
-      <c r="AX1" s="66" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="66"/>
+      <c r="AX1" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="AY1" s="66"/>
-      <c r="AZ1" s="66"/>
-      <c r="BA1" s="66"/>
-      <c r="BB1" s="66"/>
-      <c r="BC1" s="66"/>
-      <c r="BD1" s="66"/>
-      <c r="BE1" s="66"/>
-      <c r="BF1" s="66"/>
-      <c r="BG1" s="66"/>
-      <c r="BH1" s="66"/>
-      <c r="BI1" s="66"/>
-      <c r="BJ1" s="66"/>
-      <c r="BK1" s="66"/>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="66" t="s">
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="67"/>
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="BO1" s="66"/>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="66"/>
-      <c r="BR1" s="66"/>
-      <c r="BS1" s="66"/>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="66"/>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="66"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="67"/>
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="67"/>
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="66"/>
-      <c r="CH1" s="66"/>
-      <c r="CI1" s="66"/>
-      <c r="CJ1" s="66"/>
-      <c r="CK1" s="66"/>
-      <c r="CL1" s="66"/>
-      <c r="CM1" s="66"/>
-      <c r="CN1" s="66"/>
-      <c r="CO1" s="66"/>
-      <c r="CP1" s="66"/>
-      <c r="CQ1" s="66"/>
-      <c r="CR1" s="66"/>
-      <c r="CS1" s="67"/>
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="67"/>
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="67"/>
+      <c r="CS1" s="68"/>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" s="40"/>
@@ -53130,12 +54942,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03D66B45-AFBB-4B54-AE1B-19D8BA58799A}">
   <dimension ref="A1:CS43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53159,114 +54971,114 @@
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
-      <c r="K1" s="66"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="66"/>
-      <c r="N1" s="66"/>
-      <c r="O1" s="66"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="68" t="s">
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
+      <c r="M1" s="67"/>
+      <c r="N1" s="67"/>
+      <c r="O1" s="67"/>
+      <c r="P1" s="67"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="S1" s="66"/>
-      <c r="T1" s="66"/>
-      <c r="U1" s="66"/>
-      <c r="V1" s="66"/>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="66"/>
-      <c r="AA1" s="66"/>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="66"/>
-      <c r="AD1" s="66"/>
-      <c r="AE1" s="66"/>
-      <c r="AF1" s="66"/>
-      <c r="AG1" s="67"/>
-      <c r="AH1" s="63" t="s">
+      <c r="S1" s="67"/>
+      <c r="T1" s="67"/>
+      <c r="U1" s="67"/>
+      <c r="V1" s="67"/>
+      <c r="W1" s="67"/>
+      <c r="X1" s="67"/>
+      <c r="Y1" s="67"/>
+      <c r="Z1" s="67"/>
+      <c r="AA1" s="67"/>
+      <c r="AB1" s="67"/>
+      <c r="AC1" s="67"/>
+      <c r="AD1" s="67"/>
+      <c r="AE1" s="67"/>
+      <c r="AF1" s="67"/>
+      <c r="AG1" s="68"/>
+      <c r="AH1" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="AI1" s="64"/>
-      <c r="AJ1" s="64"/>
-      <c r="AK1" s="64"/>
-      <c r="AL1" s="64"/>
-      <c r="AM1" s="64"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
-      <c r="AP1" s="64"/>
-      <c r="AQ1" s="64"/>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="65"/>
-      <c r="AX1" s="66" t="s">
+      <c r="AI1" s="65"/>
+      <c r="AJ1" s="65"/>
+      <c r="AK1" s="65"/>
+      <c r="AL1" s="65"/>
+      <c r="AM1" s="65"/>
+      <c r="AN1" s="65"/>
+      <c r="AO1" s="65"/>
+      <c r="AP1" s="65"/>
+      <c r="AQ1" s="65"/>
+      <c r="AR1" s="65"/>
+      <c r="AS1" s="65"/>
+      <c r="AT1" s="65"/>
+      <c r="AU1" s="65"/>
+      <c r="AV1" s="65"/>
+      <c r="AW1" s="66"/>
+      <c r="AX1" s="67" t="s">
         <v>31</v>
       </c>
-      <c r="AY1" s="66"/>
-      <c r="AZ1" s="66"/>
-      <c r="BA1" s="66"/>
-      <c r="BB1" s="66"/>
-      <c r="BC1" s="66"/>
-      <c r="BD1" s="66"/>
-      <c r="BE1" s="66"/>
-      <c r="BF1" s="66"/>
-      <c r="BG1" s="66"/>
-      <c r="BH1" s="66"/>
-      <c r="BI1" s="66"/>
-      <c r="BJ1" s="66"/>
-      <c r="BK1" s="66"/>
-      <c r="BL1" s="66"/>
-      <c r="BM1" s="67"/>
-      <c r="BN1" s="66" t="s">
+      <c r="AY1" s="67"/>
+      <c r="AZ1" s="67"/>
+      <c r="BA1" s="67"/>
+      <c r="BB1" s="67"/>
+      <c r="BC1" s="67"/>
+      <c r="BD1" s="67"/>
+      <c r="BE1" s="67"/>
+      <c r="BF1" s="67"/>
+      <c r="BG1" s="67"/>
+      <c r="BH1" s="67"/>
+      <c r="BI1" s="67"/>
+      <c r="BJ1" s="67"/>
+      <c r="BK1" s="67"/>
+      <c r="BL1" s="67"/>
+      <c r="BM1" s="68"/>
+      <c r="BN1" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="BO1" s="66"/>
-      <c r="BP1" s="66"/>
-      <c r="BQ1" s="66"/>
-      <c r="BR1" s="66"/>
-      <c r="BS1" s="66"/>
-      <c r="BT1" s="66"/>
-      <c r="BU1" s="66"/>
-      <c r="BV1" s="66"/>
-      <c r="BW1" s="66"/>
-      <c r="BX1" s="66"/>
-      <c r="BY1" s="66"/>
-      <c r="BZ1" s="66"/>
-      <c r="CA1" s="66"/>
-      <c r="CB1" s="66"/>
-      <c r="CC1" s="67"/>
-      <c r="CD1" s="66" t="s">
+      <c r="BO1" s="67"/>
+      <c r="BP1" s="67"/>
+      <c r="BQ1" s="67"/>
+      <c r="BR1" s="67"/>
+      <c r="BS1" s="67"/>
+      <c r="BT1" s="67"/>
+      <c r="BU1" s="67"/>
+      <c r="BV1" s="67"/>
+      <c r="BW1" s="67"/>
+      <c r="BX1" s="67"/>
+      <c r="BY1" s="67"/>
+      <c r="BZ1" s="67"/>
+      <c r="CA1" s="67"/>
+      <c r="CB1" s="67"/>
+      <c r="CC1" s="68"/>
+      <c r="CD1" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="CE1" s="66"/>
-      <c r="CF1" s="66"/>
-      <c r="CG1" s="66"/>
-      <c r="CH1" s="66"/>
-      <c r="CI1" s="66"/>
-      <c r="CJ1" s="66"/>
-      <c r="CK1" s="66"/>
-      <c r="CL1" s="66"/>
-      <c r="CM1" s="66"/>
-      <c r="CN1" s="66"/>
-      <c r="CO1" s="66"/>
-      <c r="CP1" s="66"/>
-      <c r="CQ1" s="66"/>
-      <c r="CR1" s="66"/>
-      <c r="CS1" s="67"/>
+      <c r="CE1" s="67"/>
+      <c r="CF1" s="67"/>
+      <c r="CG1" s="67"/>
+      <c r="CH1" s="67"/>
+      <c r="CI1" s="67"/>
+      <c r="CJ1" s="67"/>
+      <c r="CK1" s="67"/>
+      <c r="CL1" s="67"/>
+      <c r="CM1" s="67"/>
+      <c r="CN1" s="67"/>
+      <c r="CO1" s="67"/>
+      <c r="CP1" s="67"/>
+      <c r="CQ1" s="67"/>
+      <c r="CR1" s="67"/>
+      <c r="CS1" s="68"/>
     </row>
     <row r="2" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A2" s="40"/>
@@ -53365,7 +55177,7 @@
       <c r="CP2" s="41"/>
       <c r="CQ2" s="41"/>
       <c r="CR2" s="41"/>
-      <c r="CS2" s="58"/>
+      <c r="CS2" s="57"/>
     </row>
     <row r="3" spans="1:97" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -64101,2005 +65913,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F1448B-9046-4895-AF26-0705232310C8}">
-  <dimension ref="A1:P52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="71"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="70" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="71"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="44"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="3"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="3"/>
-    </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="G3" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="13"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" s="49" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" s="49" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A4" s="50"/>
-      <c r="B4" s="51">
-        <v>75</v>
-      </c>
-      <c r="C4" s="29">
-        <v>52</v>
-      </c>
-      <c r="D4" s="43">
-        <v>136</v>
-      </c>
-      <c r="E4" s="51">
-        <v>61</v>
-      </c>
-      <c r="F4" s="29">
-        <v>75</v>
-      </c>
-      <c r="G4" s="29">
-        <v>23</v>
-      </c>
-      <c r="I4" s="35"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="52">
-        <v>310</v>
-      </c>
-      <c r="L4" s="42">
-        <v>153</v>
-      </c>
-      <c r="M4" s="42">
-        <v>135</v>
-      </c>
-      <c r="N4" s="42">
-        <v>135</v>
-      </c>
-      <c r="O4" s="42">
-        <v>0</v>
-      </c>
-      <c r="P4" s="42">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A5" s="50"/>
-      <c r="B5" s="52">
-        <v>77</v>
-      </c>
-      <c r="C5" s="42">
-        <v>52</v>
-      </c>
-      <c r="D5" s="42">
-        <v>136</v>
-      </c>
-      <c r="E5" s="42">
-        <v>61</v>
-      </c>
-      <c r="F5" s="42">
-        <v>75</v>
-      </c>
-      <c r="G5" s="42">
-        <v>25</v>
-      </c>
-      <c r="I5" s="35"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="52">
-        <v>310</v>
-      </c>
-      <c r="L5" s="42">
-        <v>153</v>
-      </c>
-      <c r="M5" s="42">
-        <v>135</v>
-      </c>
-      <c r="N5" s="42">
-        <v>135</v>
-      </c>
-      <c r="O5" s="42">
-        <v>0</v>
-      </c>
-      <c r="P5" s="42">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="52">
-        <v>77</v>
-      </c>
-      <c r="C6" s="42">
-        <v>52</v>
-      </c>
-      <c r="D6" s="42">
-        <v>70</v>
-      </c>
-      <c r="E6" s="42">
-        <v>61</v>
-      </c>
-      <c r="F6" s="42">
-        <v>9</v>
-      </c>
-      <c r="G6" s="42">
-        <v>25</v>
-      </c>
-      <c r="I6" s="35"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="52">
-        <v>310</v>
-      </c>
-      <c r="L6" s="42">
-        <v>153</v>
-      </c>
-      <c r="M6" s="42">
-        <v>135</v>
-      </c>
-      <c r="N6" s="42">
-        <v>135</v>
-      </c>
-      <c r="O6" s="42">
-        <v>0</v>
-      </c>
-      <c r="P6" s="42">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="B7" s="52">
-        <v>21</v>
-      </c>
-      <c r="C7" s="42">
-        <v>10</v>
-      </c>
-      <c r="D7" s="42">
-        <v>30</v>
-      </c>
-      <c r="E7" s="42">
-        <v>21</v>
-      </c>
-      <c r="F7" s="42">
-        <v>9</v>
-      </c>
-      <c r="G7" s="42">
-        <v>11</v>
-      </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="52">
-        <v>90</v>
-      </c>
-      <c r="L7" s="42">
-        <v>68</v>
-      </c>
-      <c r="M7" s="42">
-        <v>218</v>
-      </c>
-      <c r="N7" s="42">
-        <v>26</v>
-      </c>
-      <c r="O7" s="42">
-        <v>192</v>
-      </c>
-      <c r="P7" s="42">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="52">
-        <v>25</v>
-      </c>
-      <c r="C8" s="42">
-        <v>14</v>
-      </c>
-      <c r="D8" s="42">
-        <v>30</v>
-      </c>
-      <c r="E8" s="42">
-        <v>21</v>
-      </c>
-      <c r="F8" s="42">
-        <v>9</v>
-      </c>
-      <c r="G8" s="42">
-        <v>11</v>
-      </c>
-      <c r="I8" s="35"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="52">
-        <v>63</v>
-      </c>
-      <c r="L8" s="42">
-        <v>102</v>
-      </c>
-      <c r="M8" s="42">
-        <v>127</v>
-      </c>
-      <c r="N8" s="42">
-        <v>55</v>
-      </c>
-      <c r="O8" s="42">
-        <v>64</v>
-      </c>
-      <c r="P8" s="42">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="20"/>
-      <c r="B9" s="52">
-        <v>36</v>
-      </c>
-      <c r="C9" s="42">
-        <v>16</v>
-      </c>
-      <c r="D9" s="42">
-        <v>52</v>
-      </c>
-      <c r="E9" s="42">
-        <v>21</v>
-      </c>
-      <c r="F9" s="42">
-        <v>31</v>
-      </c>
-      <c r="G9" s="42">
-        <v>20</v>
-      </c>
-      <c r="I9" s="35"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="52">
-        <v>63</v>
-      </c>
-      <c r="L9" s="42">
-        <v>87</v>
-      </c>
-      <c r="M9" s="42">
-        <v>73</v>
-      </c>
-      <c r="N9" s="42">
-        <v>40</v>
-      </c>
-      <c r="O9" s="42">
-        <v>86</v>
-      </c>
-      <c r="P9" s="42">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="20"/>
-      <c r="B10" s="52">
-        <v>66</v>
-      </c>
-      <c r="C10" s="42">
-        <v>39</v>
-      </c>
-      <c r="D10" s="42">
-        <v>70</v>
-      </c>
-      <c r="E10" s="42">
-        <v>29</v>
-      </c>
-      <c r="F10" s="42">
-        <v>41</v>
-      </c>
-      <c r="G10" s="42">
-        <v>27</v>
-      </c>
-      <c r="I10" s="35"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="52">
-        <v>63</v>
-      </c>
-      <c r="L10" s="42">
-        <v>76</v>
-      </c>
-      <c r="M10" s="42">
-        <v>73</v>
-      </c>
-      <c r="N10" s="42">
-        <v>40</v>
-      </c>
-      <c r="O10" s="42">
-        <v>86</v>
-      </c>
-      <c r="P10" s="42">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A11" s="20"/>
-      <c r="B11" s="52">
-        <v>75</v>
-      </c>
-      <c r="C11" s="42">
-        <v>48</v>
-      </c>
-      <c r="D11" s="42">
-        <v>79</v>
-      </c>
-      <c r="E11" s="42">
-        <v>29</v>
-      </c>
-      <c r="F11" s="42">
-        <v>50</v>
-      </c>
-      <c r="G11" s="42">
-        <v>27</v>
-      </c>
-      <c r="I11" s="35"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="52">
-        <v>63</v>
-      </c>
-      <c r="L11" s="42">
-        <v>79</v>
-      </c>
-      <c r="M11" s="42">
-        <v>73</v>
-      </c>
-      <c r="N11" s="42">
-        <v>43</v>
-      </c>
-      <c r="O11" s="42">
-        <v>101</v>
-      </c>
-      <c r="P11" s="42">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A12" s="20"/>
-      <c r="B12" s="52">
-        <v>82</v>
-      </c>
-      <c r="C12" s="42">
-        <v>51</v>
-      </c>
-      <c r="D12" s="42">
-        <v>100</v>
-      </c>
-      <c r="E12" s="42">
-        <v>34</v>
-      </c>
-      <c r="F12" s="42">
-        <v>66</v>
-      </c>
-      <c r="G12" s="42">
-        <v>31</v>
-      </c>
-      <c r="I12" s="35"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="52">
-        <v>41</v>
-      </c>
-      <c r="L12" s="42">
-        <v>68</v>
-      </c>
-      <c r="M12" s="42">
-        <v>52</v>
-      </c>
-      <c r="N12" s="42">
-        <v>43</v>
-      </c>
-      <c r="O12" s="42">
-        <v>80</v>
-      </c>
-      <c r="P12" s="42">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="20"/>
-      <c r="B13" s="52">
-        <v>103</v>
-      </c>
-      <c r="C13" s="42">
-        <v>67</v>
-      </c>
-      <c r="D13" s="42">
-        <v>114</v>
-      </c>
-      <c r="E13" s="42">
-        <v>41</v>
-      </c>
-      <c r="F13" s="42">
-        <v>73</v>
-      </c>
-      <c r="G13" s="42">
-        <v>36</v>
-      </c>
-      <c r="I13" s="35"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="52">
-        <v>41</v>
-      </c>
-      <c r="L13" s="42">
-        <v>68</v>
-      </c>
-      <c r="M13" s="42">
-        <v>52</v>
-      </c>
-      <c r="N13" s="42">
-        <v>43</v>
-      </c>
-      <c r="O13" s="42">
-        <v>80</v>
-      </c>
-      <c r="P13" s="42">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A14" s="20"/>
-      <c r="B14" s="52">
-        <v>118</v>
-      </c>
-      <c r="C14" s="42">
-        <v>77</v>
-      </c>
-      <c r="D14" s="42">
-        <v>114</v>
-      </c>
-      <c r="E14" s="42">
-        <v>41</v>
-      </c>
-      <c r="F14" s="42">
-        <v>73</v>
-      </c>
-      <c r="G14" s="42">
-        <v>41</v>
-      </c>
-      <c r="I14" s="35"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="52">
-        <v>69</v>
-      </c>
-      <c r="L14" s="42">
-        <v>89</v>
-      </c>
-      <c r="M14" s="42">
-        <v>61</v>
-      </c>
-      <c r="N14" s="42">
-        <v>50</v>
-      </c>
-      <c r="O14" s="42">
-        <v>99</v>
-      </c>
-      <c r="P14" s="42">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A15" s="20"/>
-      <c r="B15" s="52">
-        <v>130</v>
-      </c>
-      <c r="C15" s="42">
-        <v>77</v>
-      </c>
-      <c r="D15" s="42">
-        <v>125</v>
-      </c>
-      <c r="E15" s="42">
-        <v>52</v>
-      </c>
-      <c r="F15" s="42">
-        <v>73</v>
-      </c>
-      <c r="G15" s="42">
-        <v>53</v>
-      </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="52">
-        <v>69</v>
-      </c>
-      <c r="L15" s="42">
-        <v>89</v>
-      </c>
-      <c r="M15" s="42">
-        <v>61</v>
-      </c>
-      <c r="N15" s="42">
-        <v>50</v>
-      </c>
-      <c r="O15" s="42">
-        <v>99</v>
-      </c>
-      <c r="P15" s="42">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="20"/>
-      <c r="B16" s="52">
-        <v>130</v>
-      </c>
-      <c r="C16" s="42">
-        <v>77</v>
-      </c>
-      <c r="D16" s="42">
-        <v>125</v>
-      </c>
-      <c r="E16" s="42">
-        <v>52</v>
-      </c>
-      <c r="F16" s="42">
-        <v>73</v>
-      </c>
-      <c r="G16" s="42">
-        <v>53</v>
-      </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="52">
-        <v>69</v>
-      </c>
-      <c r="L16" s="42">
-        <v>89</v>
-      </c>
-      <c r="M16" s="42">
-        <v>61</v>
-      </c>
-      <c r="N16" s="42">
-        <v>50</v>
-      </c>
-      <c r="O16" s="42">
-        <v>85</v>
-      </c>
-      <c r="P16" s="42">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="20"/>
-      <c r="B17" s="52">
-        <v>137</v>
-      </c>
-      <c r="C17" s="42">
-        <v>84</v>
-      </c>
-      <c r="D17" s="42">
-        <v>148</v>
-      </c>
-      <c r="E17" s="42">
-        <v>62</v>
-      </c>
-      <c r="F17" s="42">
-        <v>86</v>
-      </c>
-      <c r="G17" s="42">
-        <v>53</v>
-      </c>
-      <c r="I17" s="35"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="52">
-        <v>69</v>
-      </c>
-      <c r="L17" s="42">
-        <v>89</v>
-      </c>
-      <c r="M17" s="42">
-        <v>66</v>
-      </c>
-      <c r="N17" s="42">
-        <v>50</v>
-      </c>
-      <c r="O17" s="42">
-        <v>85</v>
-      </c>
-      <c r="P17" s="42">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="20"/>
-      <c r="B18" s="52">
-        <v>137</v>
-      </c>
-      <c r="C18" s="42">
-        <v>84</v>
-      </c>
-      <c r="D18" s="42">
-        <v>148</v>
-      </c>
-      <c r="E18" s="42">
-        <v>62</v>
-      </c>
-      <c r="F18" s="42">
-        <v>86</v>
-      </c>
-      <c r="G18" s="42">
-        <v>53</v>
-      </c>
-      <c r="I18" s="35"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="52">
-        <v>82</v>
-      </c>
-      <c r="L18" s="42">
-        <v>75</v>
-      </c>
-      <c r="M18" s="42">
-        <v>61</v>
-      </c>
-      <c r="N18" s="42">
-        <v>50</v>
-      </c>
-      <c r="O18" s="42">
-        <v>85</v>
-      </c>
-      <c r="P18" s="42">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
-      <c r="B19" s="52">
-        <v>142</v>
-      </c>
-      <c r="C19" s="42">
-        <v>89</v>
-      </c>
-      <c r="D19" s="42">
-        <v>148</v>
-      </c>
-      <c r="E19" s="42">
-        <v>62</v>
-      </c>
-      <c r="F19" s="42">
-        <v>86</v>
-      </c>
-      <c r="G19" s="42">
-        <v>53</v>
-      </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="52">
-        <v>82</v>
-      </c>
-      <c r="L19" s="42">
-        <v>75</v>
-      </c>
-      <c r="M19" s="42">
-        <v>61</v>
-      </c>
-      <c r="N19" s="42">
-        <v>50</v>
-      </c>
-      <c r="O19" s="42">
-        <v>85</v>
-      </c>
-      <c r="P19" s="42">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
-      <c r="B20" s="52">
-        <v>142</v>
-      </c>
-      <c r="C20" s="42">
-        <v>89</v>
-      </c>
-      <c r="D20" s="42">
-        <v>148</v>
-      </c>
-      <c r="E20" s="42">
-        <v>62</v>
-      </c>
-      <c r="F20" s="42">
-        <v>86</v>
-      </c>
-      <c r="G20" s="42">
-        <v>53</v>
-      </c>
-      <c r="I20" s="35"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="52">
-        <v>82</v>
-      </c>
-      <c r="L20" s="42">
-        <v>85</v>
-      </c>
-      <c r="M20" s="42">
-        <v>88</v>
-      </c>
-      <c r="N20" s="42">
-        <v>55</v>
-      </c>
-      <c r="O20" s="42">
-        <v>89</v>
-      </c>
-      <c r="P20" s="42">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="20"/>
-      <c r="B21" s="52">
-        <v>147</v>
-      </c>
-      <c r="C21" s="42">
-        <v>89</v>
-      </c>
-      <c r="D21" s="42">
-        <v>148</v>
-      </c>
-      <c r="E21" s="42">
-        <v>62</v>
-      </c>
-      <c r="F21" s="42">
-        <v>86</v>
-      </c>
-      <c r="G21" s="42">
-        <v>58</v>
-      </c>
-      <c r="I21" s="35"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="52">
-        <v>53</v>
-      </c>
-      <c r="L21" s="42">
-        <v>86</v>
-      </c>
-      <c r="M21" s="42">
-        <v>61</v>
-      </c>
-      <c r="N21" s="42">
-        <v>61</v>
-      </c>
-      <c r="O21" s="42">
-        <v>95</v>
-      </c>
-      <c r="P21" s="42">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="20"/>
-      <c r="B22" s="52">
-        <v>137</v>
-      </c>
-      <c r="C22" s="42">
-        <v>79</v>
-      </c>
-      <c r="D22" s="42">
-        <v>137</v>
-      </c>
-      <c r="E22" s="42">
-        <v>62</v>
-      </c>
-      <c r="F22" s="42">
-        <v>75</v>
-      </c>
-      <c r="G22" s="42">
-        <v>58</v>
-      </c>
-      <c r="I22" s="35"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="52">
-        <v>53</v>
-      </c>
-      <c r="L22" s="42">
-        <v>86</v>
-      </c>
-      <c r="M22" s="42">
-        <v>61</v>
-      </c>
-      <c r="N22" s="42">
-        <v>64</v>
-      </c>
-      <c r="O22" s="42">
-        <v>95</v>
-      </c>
-      <c r="P22" s="42">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A23" s="20"/>
-      <c r="B23" s="52">
-        <v>137</v>
-      </c>
-      <c r="C23" s="42">
-        <v>79</v>
-      </c>
-      <c r="D23" s="42">
-        <v>125</v>
-      </c>
-      <c r="E23" s="42">
-        <v>50</v>
-      </c>
-      <c r="F23" s="42">
-        <v>75</v>
-      </c>
-      <c r="G23" s="42">
-        <v>58</v>
-      </c>
-      <c r="I23" s="35"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="52">
-        <v>53</v>
-      </c>
-      <c r="L23" s="42">
-        <v>91</v>
-      </c>
-      <c r="M23" s="42">
-        <v>61</v>
-      </c>
-      <c r="N23" s="42">
-        <v>64</v>
-      </c>
-      <c r="O23" s="42">
-        <v>131</v>
-      </c>
-      <c r="P23" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A24" s="20"/>
-      <c r="B24" s="52">
-        <v>137</v>
-      </c>
-      <c r="C24" s="42">
-        <v>79</v>
-      </c>
-      <c r="D24" s="42">
-        <v>130</v>
-      </c>
-      <c r="E24" s="42">
-        <v>50</v>
-      </c>
-      <c r="F24" s="42">
-        <v>80</v>
-      </c>
-      <c r="G24" s="42">
-        <v>58</v>
-      </c>
-      <c r="I24" s="35"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="52">
-        <v>53</v>
-      </c>
-      <c r="L24" s="42">
-        <v>91</v>
-      </c>
-      <c r="M24" s="42">
-        <v>61</v>
-      </c>
-      <c r="N24" s="42">
-        <v>64</v>
-      </c>
-      <c r="O24" s="42">
-        <v>109</v>
-      </c>
-      <c r="P24" s="42">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A25" s="20"/>
-      <c r="B25" s="52">
-        <v>137</v>
-      </c>
-      <c r="C25" s="42">
-        <v>79</v>
-      </c>
-      <c r="D25" s="42">
-        <v>135</v>
-      </c>
-      <c r="E25" s="42">
-        <v>55</v>
-      </c>
-      <c r="F25" s="42">
-        <v>80</v>
-      </c>
-      <c r="G25" s="42">
-        <v>58</v>
-      </c>
-      <c r="I25" s="35"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="52">
-        <v>53</v>
-      </c>
-      <c r="L25" s="42">
-        <v>91</v>
-      </c>
-      <c r="M25" s="42">
-        <v>61</v>
-      </c>
-      <c r="N25" s="42">
-        <v>64</v>
-      </c>
-      <c r="O25" s="42">
-        <v>114</v>
-      </c>
-      <c r="P25" s="42">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A26" s="20"/>
-      <c r="B26" s="52">
-        <v>127</v>
-      </c>
-      <c r="C26" s="42">
-        <v>69</v>
-      </c>
-      <c r="D26" s="42">
-        <v>135</v>
-      </c>
-      <c r="E26" s="42">
-        <v>55</v>
-      </c>
-      <c r="F26" s="42">
-        <v>80</v>
-      </c>
-      <c r="G26" s="42">
-        <v>58</v>
-      </c>
-      <c r="I26" s="35"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="52">
-        <v>53</v>
-      </c>
-      <c r="L26" s="42">
-        <v>105</v>
-      </c>
-      <c r="M26" s="42">
-        <v>41</v>
-      </c>
-      <c r="N26" s="42">
-        <v>64</v>
-      </c>
-      <c r="O26" s="42">
-        <v>94</v>
-      </c>
-      <c r="P26" s="42">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A27" s="20"/>
-      <c r="B27" s="52">
-        <v>115</v>
-      </c>
-      <c r="C27" s="42">
-        <v>57</v>
-      </c>
-      <c r="D27" s="42">
-        <v>135</v>
-      </c>
-      <c r="E27" s="42">
-        <v>55</v>
-      </c>
-      <c r="F27" s="42">
-        <v>80</v>
-      </c>
-      <c r="G27" s="42">
-        <v>58</v>
-      </c>
-      <c r="I27" s="35"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="52">
-        <v>53</v>
-      </c>
-      <c r="L27" s="42">
-        <v>112</v>
-      </c>
-      <c r="M27" s="42">
-        <v>41</v>
-      </c>
-      <c r="N27" s="42">
-        <v>66</v>
-      </c>
-      <c r="O27" s="42">
-        <v>105</v>
-      </c>
-      <c r="P27" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A28" s="20"/>
-      <c r="B28" s="52">
-        <v>108</v>
-      </c>
-      <c r="C28" s="42">
-        <v>50</v>
-      </c>
-      <c r="D28" s="42">
-        <v>124</v>
-      </c>
-      <c r="E28" s="42">
-        <v>55</v>
-      </c>
-      <c r="F28" s="42">
-        <v>69</v>
-      </c>
-      <c r="G28" s="42">
-        <v>58</v>
-      </c>
-      <c r="I28" s="35"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="52">
-        <v>53</v>
-      </c>
-      <c r="L28" s="42">
-        <v>112</v>
-      </c>
-      <c r="M28" s="42">
-        <v>41</v>
-      </c>
-      <c r="N28" s="42">
-        <v>66</v>
-      </c>
-      <c r="O28" s="42">
-        <v>105</v>
-      </c>
-      <c r="P28" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A29" s="20"/>
-      <c r="B29" s="52">
-        <v>108</v>
-      </c>
-      <c r="C29" s="42">
-        <v>50</v>
-      </c>
-      <c r="D29" s="42">
-        <v>115</v>
-      </c>
-      <c r="E29" s="42">
-        <v>55</v>
-      </c>
-      <c r="F29" s="42">
-        <v>60</v>
-      </c>
-      <c r="G29" s="42">
-        <v>58</v>
-      </c>
-      <c r="I29" s="35"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="52">
-        <v>53</v>
-      </c>
-      <c r="L29" s="42">
-        <v>121</v>
-      </c>
-      <c r="M29" s="42">
-        <v>49</v>
-      </c>
-      <c r="N29" s="42">
-        <v>71</v>
-      </c>
-      <c r="O29" s="42">
-        <v>119</v>
-      </c>
-      <c r="P29" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A30" s="20"/>
-      <c r="B30" s="52">
-        <v>96</v>
-      </c>
-      <c r="C30" s="42">
-        <v>45</v>
-      </c>
-      <c r="D30" s="42">
-        <v>84</v>
-      </c>
-      <c r="E30" s="42">
-        <v>48</v>
-      </c>
-      <c r="F30" s="42">
-        <v>36</v>
-      </c>
-      <c r="G30" s="42">
-        <v>51</v>
-      </c>
-      <c r="I30" s="35"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="52">
-        <v>53</v>
-      </c>
-      <c r="L30" s="42">
-        <v>121</v>
-      </c>
-      <c r="M30" s="42">
-        <v>49</v>
-      </c>
-      <c r="N30" s="42">
-        <v>71</v>
-      </c>
-      <c r="O30" s="42">
-        <v>119</v>
-      </c>
-      <c r="P30" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="20"/>
-      <c r="B31" s="52">
-        <v>96</v>
-      </c>
-      <c r="C31" s="42">
-        <v>45</v>
-      </c>
-      <c r="D31" s="42">
-        <v>84</v>
-      </c>
-      <c r="E31" s="42">
-        <v>48</v>
-      </c>
-      <c r="F31" s="42">
-        <v>36</v>
-      </c>
-      <c r="G31" s="42">
-        <v>51</v>
-      </c>
-      <c r="I31" s="35"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="52">
-        <v>53</v>
-      </c>
-      <c r="L31" s="42">
-        <v>121</v>
-      </c>
-      <c r="M31" s="42">
-        <v>49</v>
-      </c>
-      <c r="N31" s="42">
-        <v>71</v>
-      </c>
-      <c r="O31" s="42">
-        <v>119</v>
-      </c>
-      <c r="P31" s="42">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="20"/>
-      <c r="B32" s="52">
-        <v>100</v>
-      </c>
-      <c r="C32" s="42">
-        <v>49</v>
-      </c>
-      <c r="D32" s="42">
-        <v>87</v>
-      </c>
-      <c r="E32" s="42">
-        <v>48</v>
-      </c>
-      <c r="F32" s="42">
-        <v>39</v>
-      </c>
-      <c r="G32" s="42">
-        <v>51</v>
-      </c>
-      <c r="I32" s="35"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="52">
-        <v>53</v>
-      </c>
-      <c r="L32" s="42">
-        <v>121</v>
-      </c>
-      <c r="M32" s="42">
-        <v>49</v>
-      </c>
-      <c r="N32" s="42">
-        <v>71</v>
-      </c>
-      <c r="O32" s="42">
-        <v>95</v>
-      </c>
-      <c r="P32" s="42">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A33" s="20"/>
-      <c r="B33" s="52">
-        <v>100</v>
-      </c>
-      <c r="C33" s="42">
-        <v>49</v>
-      </c>
-      <c r="D33" s="42">
-        <v>87</v>
-      </c>
-      <c r="E33" s="42">
-        <v>48</v>
-      </c>
-      <c r="F33" s="42">
-        <v>39</v>
-      </c>
-      <c r="G33" s="42">
-        <v>51</v>
-      </c>
-      <c r="I33" s="35"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="52">
-        <v>53</v>
-      </c>
-      <c r="L33" s="42">
-        <v>121</v>
-      </c>
-      <c r="M33" s="42">
-        <v>49</v>
-      </c>
-      <c r="N33" s="42">
-        <v>71</v>
-      </c>
-      <c r="O33" s="42">
-        <v>83</v>
-      </c>
-      <c r="P33" s="42">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A34" s="20"/>
-      <c r="B34" s="52">
-        <v>100</v>
-      </c>
-      <c r="C34" s="42">
-        <v>49</v>
-      </c>
-      <c r="D34" s="42">
-        <v>90</v>
-      </c>
-      <c r="E34" s="42">
-        <v>48</v>
-      </c>
-      <c r="F34" s="42">
-        <v>42</v>
-      </c>
-      <c r="G34" s="42">
-        <v>51</v>
-      </c>
-      <c r="I34" s="35"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="52">
-        <v>53</v>
-      </c>
-      <c r="L34" s="42">
-        <v>124</v>
-      </c>
-      <c r="M34" s="42">
-        <v>89</v>
-      </c>
-      <c r="N34" s="42">
-        <v>71</v>
-      </c>
-      <c r="O34" s="42">
-        <v>83</v>
-      </c>
-      <c r="P34" s="42">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A35" s="20"/>
-      <c r="B35" s="52">
-        <v>100</v>
-      </c>
-      <c r="C35" s="42">
-        <v>49</v>
-      </c>
-      <c r="D35" s="42">
-        <v>99</v>
-      </c>
-      <c r="E35" s="42">
-        <v>52</v>
-      </c>
-      <c r="F35" s="42">
-        <v>47</v>
-      </c>
-      <c r="G35" s="42">
-        <v>51</v>
-      </c>
-      <c r="I35" s="35"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="52">
-        <v>53</v>
-      </c>
-      <c r="L35" s="42">
-        <v>124</v>
-      </c>
-      <c r="M35" s="42">
-        <v>89</v>
-      </c>
-      <c r="N35" s="42">
-        <v>71</v>
-      </c>
-      <c r="O35" s="42">
-        <v>83</v>
-      </c>
-      <c r="P35" s="42">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A36" s="20"/>
-      <c r="B36" s="52">
-        <v>104</v>
-      </c>
-      <c r="C36" s="42">
-        <v>53</v>
-      </c>
-      <c r="D36" s="42">
-        <v>99</v>
-      </c>
-      <c r="E36" s="42">
-        <v>52</v>
-      </c>
-      <c r="F36" s="42">
-        <v>47</v>
-      </c>
-      <c r="G36" s="42">
-        <v>51</v>
-      </c>
-      <c r="I36" s="35"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="52">
-        <v>53</v>
-      </c>
-      <c r="L36" s="42">
-        <v>137</v>
-      </c>
-      <c r="M36" s="42">
-        <v>89</v>
-      </c>
-      <c r="N36" s="42">
-        <v>84</v>
-      </c>
-      <c r="O36" s="42">
-        <v>83</v>
-      </c>
-      <c r="P36" s="42">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A37" s="20"/>
-      <c r="B37" s="52">
-        <v>107</v>
-      </c>
-      <c r="C37" s="42">
-        <v>53</v>
-      </c>
-      <c r="D37" s="42">
-        <v>99</v>
-      </c>
-      <c r="E37" s="42">
-        <v>52</v>
-      </c>
-      <c r="F37" s="42">
-        <v>47</v>
-      </c>
-      <c r="G37" s="42">
-        <v>54</v>
-      </c>
-      <c r="I37" s="35"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="52">
-        <v>53</v>
-      </c>
-      <c r="L37" s="42">
-        <v>137</v>
-      </c>
-      <c r="M37" s="42">
-        <v>89</v>
-      </c>
-      <c r="N37" s="42">
-        <v>84</v>
-      </c>
-      <c r="O37" s="42">
-        <v>77</v>
-      </c>
-      <c r="P37" s="42">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A38" s="20"/>
-      <c r="B38" s="52">
-        <v>107</v>
-      </c>
-      <c r="C38" s="42">
-        <v>53</v>
-      </c>
-      <c r="D38" s="42">
-        <v>92</v>
-      </c>
-      <c r="E38" s="42">
-        <v>45</v>
-      </c>
-      <c r="F38" s="42">
-        <v>47</v>
-      </c>
-      <c r="G38" s="42">
-        <v>54</v>
-      </c>
-      <c r="I38" s="35"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="52">
-        <v>53</v>
-      </c>
-      <c r="L38" s="42">
-        <v>137</v>
-      </c>
-      <c r="M38" s="42">
-        <v>89</v>
-      </c>
-      <c r="N38" s="42">
-        <v>84</v>
-      </c>
-      <c r="O38" s="42">
-        <v>77</v>
-      </c>
-      <c r="P38" s="42">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="22"/>
-      <c r="B39" s="53">
-        <v>107</v>
-      </c>
-      <c r="C39" s="3">
-        <v>53</v>
-      </c>
-      <c r="D39" s="3">
-        <v>92</v>
-      </c>
-      <c r="E39" s="3">
-        <v>45</v>
-      </c>
-      <c r="F39" s="3">
-        <v>47</v>
-      </c>
-      <c r="G39" s="3">
-        <v>54</v>
-      </c>
-      <c r="I39" s="35"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="52">
-        <v>53</v>
-      </c>
-      <c r="L39" s="42">
-        <v>137</v>
-      </c>
-      <c r="M39" s="42">
-        <v>89</v>
-      </c>
-      <c r="N39" s="42">
-        <v>84</v>
-      </c>
-      <c r="O39" s="42">
-        <v>77</v>
-      </c>
-      <c r="P39" s="42">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A40" s="20"/>
-      <c r="B40" s="52"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="42"/>
-      <c r="I40" s="35"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="52">
-        <v>53</v>
-      </c>
-      <c r="L40" s="42">
-        <v>137</v>
-      </c>
-      <c r="M40" s="42">
-        <v>89</v>
-      </c>
-      <c r="N40" s="42">
-        <v>84</v>
-      </c>
-      <c r="O40" s="42">
-        <v>77</v>
-      </c>
-      <c r="P40" s="42">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A41" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="54">
-        <f t="shared" ref="B41:G41" si="0">AVERAGE(B4:B39)</f>
-        <v>103.97222222222223</v>
-      </c>
-      <c r="C41" s="54">
-        <f t="shared" si="0"/>
-        <v>58.527777777777779</v>
-      </c>
-      <c r="D41" s="54">
-        <f t="shared" si="0"/>
-        <v>107.5</v>
-      </c>
-      <c r="E41" s="54">
-        <f t="shared" si="0"/>
-        <v>48.805555555555557</v>
-      </c>
-      <c r="F41" s="6">
-        <f t="shared" si="0"/>
-        <v>58.694444444444443</v>
-      </c>
-      <c r="G41" s="6">
-        <f t="shared" si="0"/>
-        <v>45.444444444444443</v>
-      </c>
-      <c r="I41" s="35"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="52">
-        <v>53</v>
-      </c>
-      <c r="L41" s="42">
-        <v>72</v>
-      </c>
-      <c r="M41" s="42">
-        <v>72</v>
-      </c>
-      <c r="N41" s="42">
-        <v>119</v>
-      </c>
-      <c r="O41" s="42">
-        <v>77</v>
-      </c>
-      <c r="P41" s="42">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="6"/>
-      <c r="G42" s="6"/>
-      <c r="I42" s="35"/>
-      <c r="J42" s="20"/>
-      <c r="K42" s="52">
-        <v>53</v>
-      </c>
-      <c r="L42" s="42">
-        <v>72</v>
-      </c>
-      <c r="M42" s="42">
-        <v>72</v>
-      </c>
-      <c r="N42" s="42">
-        <v>119</v>
-      </c>
-      <c r="O42" s="42">
-        <v>77</v>
-      </c>
-      <c r="P42" s="42">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A43" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="54">
-        <f t="shared" ref="B43:G43" si="1">_xlfn.STDEV.S(B4:B39)</f>
-        <v>32.312302929920072</v>
-      </c>
-      <c r="C43" s="54">
-        <f t="shared" si="1"/>
-        <v>20.554437979057482</v>
-      </c>
-      <c r="D43" s="54">
-        <f t="shared" si="1"/>
-        <v>32.304356185682273</v>
-      </c>
-      <c r="E43" s="54">
-        <f t="shared" si="1"/>
-        <v>12.204962560823821</v>
-      </c>
-      <c r="F43" s="6">
-        <f t="shared" si="1"/>
-        <v>23.249970131402559</v>
-      </c>
-      <c r="G43" s="6">
-        <f t="shared" si="1"/>
-        <v>14.691969515826267</v>
-      </c>
-      <c r="I43" s="35"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="52">
-        <v>37</v>
-      </c>
-      <c r="L43" s="42">
-        <v>72</v>
-      </c>
-      <c r="M43" s="42">
-        <v>49</v>
-      </c>
-      <c r="N43" s="42">
-        <v>121</v>
-      </c>
-      <c r="O43" s="42">
-        <v>77</v>
-      </c>
-      <c r="P43" s="42">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="23"/>
-      <c r="B44" s="54"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="22"/>
-      <c r="K44" s="53">
-        <v>37</v>
-      </c>
-      <c r="L44" s="3">
-        <v>72</v>
-      </c>
-      <c r="M44" s="3">
-        <v>49</v>
-      </c>
-      <c r="N44" s="3">
-        <v>90</v>
-      </c>
-      <c r="O44" s="3">
-        <v>77</v>
-      </c>
-      <c r="P44" s="3">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45" s="55">
-        <f>_xlfn.CONFIDENCE.NORM(0.05,B43,35)</f>
-        <v>10.70488436973214</v>
-      </c>
-      <c r="C45" s="55">
-        <f t="shared" ref="C45:G45" si="2">_xlfn.CONFIDENCE.NORM(0.05,C43,35)</f>
-        <v>6.8095697891869635</v>
-      </c>
-      <c r="D45" s="55">
-        <f t="shared" si="2"/>
-        <v>10.702251658025828</v>
-      </c>
-      <c r="E45" s="55">
-        <f t="shared" si="2"/>
-        <v>4.0434355060947702</v>
-      </c>
-      <c r="F45" s="55">
-        <f t="shared" si="2"/>
-        <v>7.7025844427179004</v>
-      </c>
-      <c r="G45" s="55">
-        <f t="shared" si="2"/>
-        <v>4.8673669336306489</v>
-      </c>
-      <c r="I45" s="35"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="52"/>
-      <c r="L45" s="52"/>
-      <c r="M45" s="52"/>
-      <c r="N45" s="52"/>
-      <c r="O45" s="42"/>
-      <c r="P45" s="42"/>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
-      <c r="B46" s="56"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="57"/>
-      <c r="J46" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="K46" s="54">
-        <f>AVERAGE(K4:K44)</f>
-        <v>76</v>
-      </c>
-      <c r="L46" s="54">
-        <f t="shared" ref="L46:P46" si="3">AVERAGE(L4:L44)</f>
-        <v>102.39024390243902</v>
-      </c>
-      <c r="M46" s="54">
-        <f t="shared" si="3"/>
-        <v>74.878048780487802</v>
-      </c>
-      <c r="N46" s="54">
-        <f t="shared" si="3"/>
-        <v>71.439024390243901</v>
-      </c>
-      <c r="O46" s="6">
-        <f t="shared" si="3"/>
-        <v>86.926829268292678</v>
-      </c>
-      <c r="P46" s="6">
-        <f t="shared" si="3"/>
-        <v>92.341463414634148</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="8">
-        <f>AVERAGE(B41:G41)</f>
-        <v>70.490740740740748</v>
-      </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="26"/>
-      <c r="I47" s="57"/>
-      <c r="J47" s="23"/>
-      <c r="K47" s="54"/>
-      <c r="L47" s="54"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="54"/>
-      <c r="O47" s="6"/>
-      <c r="P47" s="6"/>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="57"/>
-      <c r="J48" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="K48" s="54">
-        <f>_xlfn.STDEV.S(K4:K44)</f>
-        <v>67.559973357010733</v>
-      </c>
-      <c r="L48" s="54">
-        <f t="shared" ref="L48:P48" si="4">_xlfn.STDEV.S(L4:L44)</f>
-        <v>26.786076652601153</v>
-      </c>
-      <c r="M48" s="54">
-        <f t="shared" si="4"/>
-        <v>34.213444084125193</v>
-      </c>
-      <c r="N48" s="54">
-        <f t="shared" si="4"/>
-        <v>27.588991265075101</v>
-      </c>
-      <c r="O48" s="6">
-        <f t="shared" si="4"/>
-        <v>32.725670538510322</v>
-      </c>
-      <c r="P48" s="6">
-        <f t="shared" si="4"/>
-        <v>37.540384758348942</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A49" s="5"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="57"/>
-      <c r="J49" s="23"/>
-      <c r="K49" s="54"/>
-      <c r="L49" s="54"/>
-      <c r="M49" s="54"/>
-      <c r="N49" s="54"/>
-      <c r="O49" s="6"/>
-      <c r="P49" s="6"/>
-    </row>
-    <row r="50" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="5"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="26"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="K50" s="55">
-        <f>_xlfn.CONFIDENCE.NORM(0.05,K48,40)</f>
-        <v>20.936667934651886</v>
-      </c>
-      <c r="L50" s="55">
-        <f t="shared" ref="L50:P50" si="5">_xlfn.CONFIDENCE.NORM(0.05,L48,40)</f>
-        <v>8.3009386221056936</v>
-      </c>
-      <c r="M50" s="55">
-        <f t="shared" si="5"/>
-        <v>10.602661340685339</v>
-      </c>
-      <c r="N50" s="55">
-        <f t="shared" si="5"/>
-        <v>8.5497598661937424</v>
-      </c>
-      <c r="O50" s="8">
-        <f t="shared" si="5"/>
-        <v>10.141604014302219</v>
-      </c>
-      <c r="P50" s="8">
-        <f t="shared" si="5"/>
-        <v>11.633671992013273</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="5"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="26"/>
-      <c r="I51" s="57"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="56"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
-      <c r="P51" s="5"/>
-    </row>
-    <row r="52" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="26"/>
-      <c r="I52" s="57"/>
-      <c r="J52" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="K52" s="8">
-        <f>AVERAGE(K46:P46)</f>
-        <v>83.995934959349597</v>
-      </c>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
-      <c r="P52" s="5"/>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="J1:P1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>